<commit_message>
added the ability to compare the raw and matched data using multiple linear regression
</commit_message>
<xml_diff>
--- a/Data/timings_both_models_4-4_treatments.xlsx
+++ b/Data/timings_both_models_4-4_treatments.xlsx
@@ -464,25 +464,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1.11</v>
+        <v>0.507</v>
       </c>
       <c r="G2">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H2">
-        <v>0.46</v>
+        <v>0.227</v>
       </c>
       <c r="I2">
-        <v>0.27</v>
+        <v>0.127</v>
       </c>
       <c r="J2">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00026</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -502,25 +502,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1.04</v>
+        <v>0.517</v>
       </c>
       <c r="G3">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H3">
-        <v>0.47</v>
+        <v>0.238</v>
       </c>
       <c r="I3">
-        <v>0.26</v>
+        <v>0.132</v>
       </c>
       <c r="J3">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -540,25 +540,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>1.05</v>
+        <v>0.515</v>
       </c>
       <c r="G4">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H4">
-        <v>0.47</v>
+        <v>0.235</v>
       </c>
       <c r="I4">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="J4">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00021</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -578,25 +578,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>1.06</v>
+        <v>0.518</v>
       </c>
       <c r="G5">
-        <v>0.02</v>
+        <v>0.008</v>
       </c>
       <c r="H5">
-        <v>0.46</v>
+        <v>0.235</v>
       </c>
       <c r="I5">
-        <v>0.28</v>
+        <v>0.129</v>
       </c>
       <c r="J5">
-        <v>0.27</v>
+        <v>0.133</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.0003</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -616,25 +616,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>1.05</v>
+        <v>0.515</v>
       </c>
       <c r="G6">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H6">
-        <v>0.48</v>
+        <v>0.237</v>
       </c>
       <c r="I6">
-        <v>0.26</v>
+        <v>0.129</v>
       </c>
       <c r="J6">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00032</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -654,25 +654,25 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1.04</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="G7">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H7">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="I7">
-        <v>0.26</v>
+        <v>0.17</v>
       </c>
       <c r="J7">
-        <v>0.27</v>
+        <v>0.127</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.0003</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -692,25 +692,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>1.09</v>
+        <v>0.509</v>
       </c>
       <c r="G8">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="H8">
-        <v>0.47</v>
+        <v>0.236</v>
       </c>
       <c r="I8">
-        <v>0.26</v>
+        <v>0.126</v>
       </c>
       <c r="J8">
-        <v>0.32</v>
+        <v>0.126</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00029</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -730,25 +730,25 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>1.05</v>
+        <v>0.518</v>
       </c>
       <c r="G9">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H9">
-        <v>0.46</v>
+        <v>0.237</v>
       </c>
       <c r="I9">
-        <v>0.27</v>
+        <v>0.128</v>
       </c>
       <c r="J9">
-        <v>0.26</v>
+        <v>0.133</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00025</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -768,25 +768,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>1.04</v>
+        <v>0.498</v>
       </c>
       <c r="G10">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H10">
-        <v>0.46</v>
+        <v>0.228</v>
       </c>
       <c r="I10">
-        <v>0.27</v>
+        <v>0.125</v>
       </c>
       <c r="J10">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.00035</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -806,25 +806,25 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>1.05</v>
+        <v>0.504</v>
       </c>
       <c r="G11">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H11">
-        <v>0.47</v>
+        <v>0.234</v>
       </c>
       <c r="I11">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="J11">
-        <v>0.28</v>
+        <v>0.124</v>
       </c>
       <c r="K11">
         <v>1000</v>
       </c>
       <c r="L11">
-        <v>0.0002</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -844,25 +844,25 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1.02</v>
+        <v>0.516</v>
       </c>
       <c r="G12">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="H12">
-        <v>0.46</v>
+        <v>0.234</v>
       </c>
       <c r="I12">
-        <v>0.26</v>
+        <v>0.131</v>
       </c>
       <c r="J12">
-        <v>0.26</v>
+        <v>0.131</v>
       </c>
       <c r="K12">
         <v>1000</v>
       </c>
       <c r="L12">
-        <v>0.00017</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -882,25 +882,25 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>1.03</v>
+        <v>0.51</v>
       </c>
       <c r="G13">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H13">
-        <v>0.46</v>
+        <v>0.234</v>
       </c>
       <c r="I13">
-        <v>0.27</v>
+        <v>0.128</v>
       </c>
       <c r="J13">
-        <v>0.26</v>
+        <v>0.128</v>
       </c>
       <c r="K13">
         <v>1000</v>
       </c>
       <c r="L13">
-        <v>0.00024</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -920,25 +920,25 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>1.05</v>
+        <v>0.517</v>
       </c>
       <c r="G14">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H14">
-        <v>0.48</v>
+        <v>0.239</v>
       </c>
       <c r="I14">
-        <v>0.26</v>
+        <v>0.129</v>
       </c>
       <c r="J14">
-        <v>0.27</v>
+        <v>0.129</v>
       </c>
       <c r="K14">
         <v>1000</v>
       </c>
       <c r="L14">
-        <v>0.00039</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -958,25 +958,25 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>1.05</v>
+        <v>0.507</v>
       </c>
       <c r="G15">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H15">
-        <v>0.47</v>
+        <v>0.232</v>
       </c>
       <c r="I15">
-        <v>0.28</v>
+        <v>0.124</v>
       </c>
       <c r="J15">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="K15">
         <v>1000</v>
       </c>
       <c r="L15">
-        <v>0.00025</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -996,25 +996,25 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>1.04</v>
+        <v>0.513</v>
       </c>
       <c r="G16">
-        <v>0.02</v>
+        <v>0.008</v>
       </c>
       <c r="H16">
-        <v>0.45</v>
+        <v>0.233</v>
       </c>
       <c r="I16">
-        <v>0.27</v>
+        <v>0.125</v>
       </c>
       <c r="J16">
-        <v>0.27</v>
+        <v>0.134</v>
       </c>
       <c r="K16">
         <v>1000</v>
       </c>
       <c r="L16">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
   </sheetData>
@@ -1082,25 +1082,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2.15</v>
+        <v>1.053</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I2">
-        <v>0.6899999999999999</v>
+        <v>0.352</v>
       </c>
       <c r="J2">
-        <v>0.68</v>
+        <v>0.355</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00027</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1120,25 +1120,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2.15</v>
+        <v>1.057</v>
       </c>
       <c r="G3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I3">
-        <v>0.68</v>
+        <v>0.347</v>
       </c>
       <c r="J3">
-        <v>0.68</v>
+        <v>0.37</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00045</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1158,25 +1158,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2.17</v>
+        <v>1.05</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I4">
-        <v>0.6899999999999999</v>
+        <v>0.354</v>
       </c>
       <c r="J4">
-        <v>0.7</v>
+        <v>0.358</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00024</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1196,25 +1196,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>2.17</v>
+        <v>1.045</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I5">
-        <v>0.6899999999999999</v>
+        <v>0.351</v>
       </c>
       <c r="J5">
-        <v>0.68</v>
+        <v>0.362</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.0003</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1234,25 +1234,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>2.15</v>
+        <v>1.043</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I6">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="J6">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00027</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1272,25 +1272,25 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>2.16</v>
+        <v>1.05</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I7">
-        <v>0.6899999999999999</v>
+        <v>0.353</v>
       </c>
       <c r="J7">
-        <v>0.68</v>
+        <v>0.353</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.00016</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1310,25 +1310,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>2.15</v>
+        <v>1.034</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I8">
-        <v>0.6899999999999999</v>
+        <v>0.349</v>
       </c>
       <c r="J8">
-        <v>0.68</v>
+        <v>0.347</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00018</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1348,25 +1348,25 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>2.14</v>
+        <v>1.04</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I9">
-        <v>0.67</v>
+        <v>0.346</v>
       </c>
       <c r="J9">
-        <v>0.68</v>
+        <v>0.354</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00026</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1386,25 +1386,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>2.17</v>
+        <v>1.064</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I10">
-        <v>0.68</v>
+        <v>0.364</v>
       </c>
       <c r="J10">
-        <v>0.7</v>
+        <v>0.368</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.0002</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1424,25 +1424,25 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>2.16</v>
+        <v>1.051</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I11">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="J11">
-        <v>0.6899999999999999</v>
+        <v>0.356</v>
       </c>
       <c r="K11">
         <v>1000</v>
       </c>
       <c r="L11">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1462,25 +1462,25 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>2.17</v>
+        <v>1.077</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I12">
-        <v>0.6899999999999999</v>
+        <v>0.376</v>
       </c>
       <c r="J12">
-        <v>0.7</v>
+        <v>0.354</v>
       </c>
       <c r="K12">
         <v>1000</v>
       </c>
       <c r="L12">
-        <v>0.00012</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1500,25 +1500,25 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>2.15</v>
+        <v>1.051</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I13">
-        <v>0.6899999999999999</v>
+        <v>0.351</v>
       </c>
       <c r="J13">
-        <v>0.68</v>
+        <v>0.355</v>
       </c>
       <c r="K13">
         <v>1000</v>
       </c>
       <c r="L13">
-        <v>0.00032</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1538,25 +1538,25 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>2.2</v>
+        <v>1.038</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I14">
-        <v>0.6899999999999999</v>
+        <v>0.345</v>
       </c>
       <c r="J14">
-        <v>0.72</v>
+        <v>0.352</v>
       </c>
       <c r="K14">
         <v>1000</v>
       </c>
       <c r="L14">
-        <v>0.00028</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1576,25 +1576,25 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>2.14</v>
+        <v>1.043</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I15">
-        <v>0.68</v>
+        <v>0.357</v>
       </c>
       <c r="J15">
-        <v>0.67</v>
+        <v>0.352</v>
       </c>
       <c r="K15">
         <v>1000</v>
       </c>
       <c r="L15">
-        <v>0.00014</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1614,25 +1614,25 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>2.14</v>
+        <v>1.036</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I16">
-        <v>0.68</v>
+        <v>0.349</v>
       </c>
       <c r="J16">
-        <v>0.68</v>
+        <v>0.358</v>
       </c>
       <c r="K16">
         <v>1000</v>
       </c>
       <c r="L16">
-        <v>0.00021</v>
+        <v>6e-05</v>
       </c>
     </row>
   </sheetData>
@@ -1700,25 +1700,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1.11</v>
+        <v>0.507</v>
       </c>
       <c r="G2">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H2">
-        <v>0.46</v>
+        <v>0.227</v>
       </c>
       <c r="I2">
-        <v>0.27</v>
+        <v>0.127</v>
       </c>
       <c r="J2">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00026</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1738,25 +1738,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1.04</v>
+        <v>0.517</v>
       </c>
       <c r="G3">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H3">
-        <v>0.47</v>
+        <v>0.238</v>
       </c>
       <c r="I3">
-        <v>0.26</v>
+        <v>0.132</v>
       </c>
       <c r="J3">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1776,25 +1776,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>1.05</v>
+        <v>0.515</v>
       </c>
       <c r="G4">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H4">
-        <v>0.47</v>
+        <v>0.235</v>
       </c>
       <c r="I4">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="J4">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00021</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1814,25 +1814,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>1.06</v>
+        <v>0.518</v>
       </c>
       <c r="G5">
-        <v>0.02</v>
+        <v>0.008</v>
       </c>
       <c r="H5">
-        <v>0.46</v>
+        <v>0.235</v>
       </c>
       <c r="I5">
-        <v>0.28</v>
+        <v>0.129</v>
       </c>
       <c r="J5">
-        <v>0.27</v>
+        <v>0.133</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.0003</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1852,25 +1852,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>1.05</v>
+        <v>0.515</v>
       </c>
       <c r="G6">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H6">
-        <v>0.48</v>
+        <v>0.237</v>
       </c>
       <c r="I6">
-        <v>0.26</v>
+        <v>0.129</v>
       </c>
       <c r="J6">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00032</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1890,25 +1890,25 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1.04</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="G7">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H7">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="I7">
-        <v>0.26</v>
+        <v>0.17</v>
       </c>
       <c r="J7">
-        <v>0.27</v>
+        <v>0.127</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.0003</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1928,25 +1928,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>1.09</v>
+        <v>0.509</v>
       </c>
       <c r="G8">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="H8">
-        <v>0.47</v>
+        <v>0.236</v>
       </c>
       <c r="I8">
-        <v>0.26</v>
+        <v>0.126</v>
       </c>
       <c r="J8">
-        <v>0.32</v>
+        <v>0.126</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00029</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1966,25 +1966,25 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>1.05</v>
+        <v>0.518</v>
       </c>
       <c r="G9">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H9">
-        <v>0.46</v>
+        <v>0.237</v>
       </c>
       <c r="I9">
-        <v>0.27</v>
+        <v>0.128</v>
       </c>
       <c r="J9">
-        <v>0.26</v>
+        <v>0.133</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00025</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2004,25 +2004,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>1.04</v>
+        <v>0.498</v>
       </c>
       <c r="G10">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H10">
-        <v>0.46</v>
+        <v>0.228</v>
       </c>
       <c r="I10">
-        <v>0.27</v>
+        <v>0.125</v>
       </c>
       <c r="J10">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.00035</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2042,25 +2042,25 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>1.05</v>
+        <v>0.504</v>
       </c>
       <c r="G11">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H11">
-        <v>0.47</v>
+        <v>0.234</v>
       </c>
       <c r="I11">
-        <v>0.26</v>
+        <v>0.125</v>
       </c>
       <c r="J11">
-        <v>0.28</v>
+        <v>0.124</v>
       </c>
       <c r="K11">
         <v>1000</v>
       </c>
       <c r="L11">
-        <v>0.0002</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2080,25 +2080,25 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1.02</v>
+        <v>0.516</v>
       </c>
       <c r="G12">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="H12">
-        <v>0.46</v>
+        <v>0.234</v>
       </c>
       <c r="I12">
-        <v>0.26</v>
+        <v>0.131</v>
       </c>
       <c r="J12">
-        <v>0.26</v>
+        <v>0.131</v>
       </c>
       <c r="K12">
         <v>1000</v>
       </c>
       <c r="L12">
-        <v>0.00017</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2118,25 +2118,25 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>1.03</v>
+        <v>0.51</v>
       </c>
       <c r="G13">
-        <v>0.02</v>
+        <v>0.007</v>
       </c>
       <c r="H13">
-        <v>0.46</v>
+        <v>0.234</v>
       </c>
       <c r="I13">
-        <v>0.27</v>
+        <v>0.128</v>
       </c>
       <c r="J13">
-        <v>0.26</v>
+        <v>0.128</v>
       </c>
       <c r="K13">
         <v>1000</v>
       </c>
       <c r="L13">
-        <v>0.00024</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2156,25 +2156,25 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>1.05</v>
+        <v>0.517</v>
       </c>
       <c r="G14">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H14">
-        <v>0.48</v>
+        <v>0.239</v>
       </c>
       <c r="I14">
-        <v>0.26</v>
+        <v>0.129</v>
       </c>
       <c r="J14">
-        <v>0.27</v>
+        <v>0.129</v>
       </c>
       <c r="K14">
         <v>1000</v>
       </c>
       <c r="L14">
-        <v>0.00039</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2194,25 +2194,25 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>1.05</v>
+        <v>0.507</v>
       </c>
       <c r="G15">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="H15">
-        <v>0.47</v>
+        <v>0.232</v>
       </c>
       <c r="I15">
-        <v>0.28</v>
+        <v>0.124</v>
       </c>
       <c r="J15">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="K15">
         <v>1000</v>
       </c>
       <c r="L15">
-        <v>0.00025</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2232,25 +2232,25 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>1.04</v>
+        <v>0.513</v>
       </c>
       <c r="G16">
-        <v>0.02</v>
+        <v>0.008</v>
       </c>
       <c r="H16">
-        <v>0.45</v>
+        <v>0.233</v>
       </c>
       <c r="I16">
-        <v>0.27</v>
+        <v>0.125</v>
       </c>
       <c r="J16">
-        <v>0.27</v>
+        <v>0.134</v>
       </c>
       <c r="K16">
         <v>1000</v>
       </c>
       <c r="L16">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2270,25 +2270,25 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>2.15</v>
+        <v>1.053</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I17">
-        <v>0.6899999999999999</v>
+        <v>0.352</v>
       </c>
       <c r="J17">
-        <v>0.68</v>
+        <v>0.355</v>
       </c>
       <c r="K17">
         <v>1000</v>
       </c>
       <c r="L17">
-        <v>0.00027</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2308,25 +2308,25 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>2.15</v>
+        <v>1.057</v>
       </c>
       <c r="G18">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I18">
-        <v>0.68</v>
+        <v>0.347</v>
       </c>
       <c r="J18">
-        <v>0.68</v>
+        <v>0.37</v>
       </c>
       <c r="K18">
         <v>1000</v>
       </c>
       <c r="L18">
-        <v>0.00045</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2346,25 +2346,25 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>2.17</v>
+        <v>1.05</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I19">
-        <v>0.6899999999999999</v>
+        <v>0.354</v>
       </c>
       <c r="J19">
-        <v>0.7</v>
+        <v>0.358</v>
       </c>
       <c r="K19">
         <v>1000</v>
       </c>
       <c r="L19">
-        <v>0.00024</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2384,25 +2384,25 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <v>2.17</v>
+        <v>1.045</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I20">
-        <v>0.6899999999999999</v>
+        <v>0.351</v>
       </c>
       <c r="J20">
-        <v>0.68</v>
+        <v>0.362</v>
       </c>
       <c r="K20">
         <v>1000</v>
       </c>
       <c r="L20">
-        <v>0.0003</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2422,25 +2422,25 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>2.15</v>
+        <v>1.043</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I21">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="J21">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="K21">
         <v>1000</v>
       </c>
       <c r="L21">
-        <v>0.00027</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2460,25 +2460,25 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>2.16</v>
+        <v>1.05</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I22">
-        <v>0.6899999999999999</v>
+        <v>0.353</v>
       </c>
       <c r="J22">
-        <v>0.68</v>
+        <v>0.353</v>
       </c>
       <c r="K22">
         <v>1000</v>
       </c>
       <c r="L22">
-        <v>0.00016</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2498,25 +2498,25 @@
         <v>2</v>
       </c>
       <c r="F23">
-        <v>2.15</v>
+        <v>1.034</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I23">
-        <v>0.6899999999999999</v>
+        <v>0.349</v>
       </c>
       <c r="J23">
-        <v>0.68</v>
+        <v>0.347</v>
       </c>
       <c r="K23">
         <v>1000</v>
       </c>
       <c r="L23">
-        <v>0.00018</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2536,25 +2536,25 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <v>2.14</v>
+        <v>1.04</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I24">
-        <v>0.67</v>
+        <v>0.346</v>
       </c>
       <c r="J24">
-        <v>0.68</v>
+        <v>0.354</v>
       </c>
       <c r="K24">
         <v>1000</v>
       </c>
       <c r="L24">
-        <v>0.00026</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2574,25 +2574,25 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>2.17</v>
+        <v>1.064</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I25">
-        <v>0.68</v>
+        <v>0.364</v>
       </c>
       <c r="J25">
-        <v>0.7</v>
+        <v>0.368</v>
       </c>
       <c r="K25">
         <v>1000</v>
       </c>
       <c r="L25">
-        <v>0.0002</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2612,25 +2612,25 @@
         <v>5</v>
       </c>
       <c r="F26">
-        <v>2.16</v>
+        <v>1.051</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I26">
-        <v>0.6899999999999999</v>
+        <v>0.355</v>
       </c>
       <c r="J26">
-        <v>0.6899999999999999</v>
+        <v>0.356</v>
       </c>
       <c r="K26">
         <v>1000</v>
       </c>
       <c r="L26">
-        <v>0.00024</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2650,25 +2650,25 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>2.17</v>
+        <v>1.077</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I27">
-        <v>0.6899999999999999</v>
+        <v>0.376</v>
       </c>
       <c r="J27">
-        <v>0.7</v>
+        <v>0.354</v>
       </c>
       <c r="K27">
         <v>1000</v>
       </c>
       <c r="L27">
-        <v>0.00012</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2688,25 +2688,25 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <v>2.15</v>
+        <v>1.051</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I28">
-        <v>0.6899999999999999</v>
+        <v>0.351</v>
       </c>
       <c r="J28">
-        <v>0.68</v>
+        <v>0.355</v>
       </c>
       <c r="K28">
         <v>1000</v>
       </c>
       <c r="L28">
-        <v>0.00032</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2726,25 +2726,25 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <v>2.2</v>
+        <v>1.038</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I29">
-        <v>0.6899999999999999</v>
+        <v>0.345</v>
       </c>
       <c r="J29">
-        <v>0.72</v>
+        <v>0.352</v>
       </c>
       <c r="K29">
         <v>1000</v>
       </c>
       <c r="L29">
-        <v>0.00028</v>
+        <v>6.999999999999999e-05</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2764,25 +2764,25 @@
         <v>4</v>
       </c>
       <c r="F30">
-        <v>2.14</v>
+        <v>1.043</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
       <c r="I30">
-        <v>0.68</v>
+        <v>0.357</v>
       </c>
       <c r="J30">
-        <v>0.67</v>
+        <v>0.352</v>
       </c>
       <c r="K30">
         <v>1000</v>
       </c>
       <c r="L30">
-        <v>0.00014</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2802,25 +2802,25 @@
         <v>5</v>
       </c>
       <c r="F31">
-        <v>2.14</v>
+        <v>1.036</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I31">
-        <v>0.68</v>
+        <v>0.349</v>
       </c>
       <c r="J31">
-        <v>0.68</v>
+        <v>0.358</v>
       </c>
       <c r="K31">
         <v>1000</v>
       </c>
       <c r="L31">
-        <v>0.00021</v>
+        <v>6e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>